<commit_message>
Finished all views, added filters, and created theme
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9702616-675D-46C0-9151-BB6CB14E03EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\GitHub\CMPG323-Project-5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCF60F-988C-4776-AFA7-3B1812DC46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34410" yWindow="3390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -322,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +352,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -795,17 +801,17 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -827,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -838,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -849,7 +855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -860,7 +866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -871,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -882,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -893,7 +899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -904,7 +910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -925,10 +931,10 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -939,7 +945,7 @@
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -985,7 +991,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="11" t="b">
         <v>1</v>
@@ -1008,7 +1014,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>44541</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>44409</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>44434</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -1180,14 +1186,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>68</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>77</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>80</v>
       </c>
@@ -1285,10 +1291,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1296,7 +1302,7 @@
     <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -1386,6 +1392,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A38BD02CE626854CB2A69241B23A3E9B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3995f0f3d16fb037e2c25f34d1e51555">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a090801-4708-43a5-9598-e4e2166c002c" xmlns:ns3="4f4a8c57-659f-4264-b765-bd165a88863b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66ec43485dfc5a4a75bbf1242e9d13e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7a090801-4708-43a5-9598-e4e2166c002c"/>
@@ -1608,34 +1634,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Cahnge made to views, added theme, and filters
</commit_message>
<xml_diff>
--- a/Connected Office Dataset.xlsx
+++ b/Connected Office Dataset.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25825"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B9702616-675D-46C0-9151-BB6CB14E03EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phill\Documents\GitHub\CMPG323-Project-5\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BCCF60F-988C-4776-AFA7-3B1812DC46D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34410" yWindow="3390" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zone" sheetId="1" r:id="rId1"/>
@@ -322,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +352,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -795,17 +801,17 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -816,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -827,7 +833,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -838,7 +844,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
@@ -849,7 +855,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
@@ -860,7 +866,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>15</v>
       </c>
@@ -871,7 +877,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -882,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>21</v>
       </c>
@@ -893,7 +899,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
@@ -904,7 +910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>27</v>
       </c>
@@ -925,10 +931,10 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
@@ -939,7 +945,7 @@
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,7 +968,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>36</v>
       </c>
@@ -985,7 +991,7 @@
         <v>43855</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>40</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="F3" s="11" t="b">
         <v>1</v>
@@ -1008,7 +1014,7 @@
         <v>44229</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -1031,7 +1037,7 @@
         <v>44541</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
@@ -1054,7 +1060,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>44641</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>52</v>
       </c>
@@ -1100,7 +1106,7 @@
         <v>44333</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>55</v>
       </c>
@@ -1123,7 +1129,7 @@
         <v>44409</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>56</v>
       </c>
@@ -1146,7 +1152,7 @@
         <v>44434</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>58</v>
       </c>
@@ -1180,14 +1186,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>62</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>65</v>
       </c>
@@ -1220,7 +1226,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>68</v>
       </c>
@@ -1231,7 +1237,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>71</v>
       </c>
@@ -1242,7 +1248,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>74</v>
       </c>
@@ -1253,7 +1259,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>77</v>
       </c>
@@ -1264,7 +1270,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>80</v>
       </c>
@@ -1285,10 +1291,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1296,7 +1302,7 @@
     <col min="4" max="4" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1310,7 +1316,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>85</v>
       </c>
@@ -1324,7 +1330,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>87</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>89</v>
       </c>
@@ -1352,7 +1358,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>91</v>
       </c>
@@ -1366,7 +1372,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>93</v>
       </c>
@@ -1386,6 +1392,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A38BD02CE626854CB2A69241B23A3E9B" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3995f0f3d16fb037e2c25f34d1e51555">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7a090801-4708-43a5-9598-e4e2166c002c" xmlns:ns3="4f4a8c57-659f-4264-b765-bd165a88863b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="66ec43485dfc5a4a75bbf1242e9d13e6" ns2:_="" ns3:_="">
     <xsd:import namespace="7a090801-4708-43a5-9598-e4e2166c002c"/>
@@ -1608,34 +1634,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7a090801-4708-43a5-9598-e4e2166c002c">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="4f4a8c57-659f-4264-b765-bd165a88863b" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8B45281D-5D5A-4087-8014-4B4FA16E83A5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0A227DC9-4D6F-4F55-89DE-623758C7FB72}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9B6EE518-5DC1-4AFD-B150-7E05CC0C76D1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="7a090801-4708-43a5-9598-e4e2166c002c"/>
+    <ds:schemaRef ds:uri="4f4a8c57-659f-4264-b765-bd165a88863b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>